<commit_message>
Change compass colours to red (left, port) green (right, starboard)
</commit_message>
<xml_diff>
--- a/inst/extdata/compass.xlsx
+++ b/inst/extdata/compass.xlsx
@@ -646,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -673,268 +673,259 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4221,9 +4212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="130" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4244,789 +4233,789 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49"/>
-      <c r="AA1" s="49"/>
-      <c r="AB1" s="49"/>
-      <c r="AC1" s="46"/>
+      <c r="A1" s="12"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
+      <c r="AC1" s="12"/>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="44" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="33" t="s">
+      <c r="H2" s="44"/>
+      <c r="I2" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="41" t="s">
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="45"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
       <c r="R2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="44" t="s">
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="W2" s="18"/>
-      <c r="X2" s="33" t="s">
+      <c r="W2" s="44"/>
+      <c r="X2" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="46"/>
+      <c r="Y2" s="12"/>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="20" t="s">
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="19"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="16" t="s">
+      <c r="H3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="62"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="46"/>
-      <c r="P3" s="46"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
       <c r="Q3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="47" t="s">
+      <c r="R3" s="13" t="s">
         <v>12</v>
       </c>
       <c r="S3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="46"/>
-      <c r="U3" s="46"/>
-      <c r="V3" s="20" t="s">
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="W3" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="46"/>
+      <c r="W3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="X3" s="62"/>
+      <c r="Y3" s="12"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="21" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="34"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="35" t="s">
+      <c r="I4" s="64"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="17"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="46"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
       <c r="R4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="S4" s="46"/>
-      <c r="T4" s="46"/>
-      <c r="U4" s="46"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="21" t="s">
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="60"/>
+      <c r="W4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="46"/>
+      <c r="X4" s="64"/>
+      <c r="Y4" s="12"/>
     </row>
     <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
-      <c r="J5" s="46"/>
-      <c r="K5" s="46"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="46"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="46"/>
-      <c r="Q5" s="46"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="46"/>
-      <c r="T5" s="46"/>
-      <c r="U5" s="46"/>
-      <c r="V5" s="46"/>
-      <c r="W5" s="46"/>
-      <c r="X5" s="46"/>
-      <c r="Y5" s="46"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
     </row>
     <row r="6" spans="1:29" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="51" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="51" t="s">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="98" t="s">
+      <c r="H6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="96"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="97" t="s">
+      <c r="I6" s="37"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="53" t="s">
+      <c r="N6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="O6" s="46"/>
-      <c r="P6" s="46"/>
-      <c r="Q6" s="51" t="s">
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="R6" s="52" t="s">
+      <c r="R6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="S6" s="53" t="s">
+      <c r="S6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="T6" s="49"/>
-      <c r="U6" s="49"/>
-      <c r="V6" s="51" t="s">
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="W6" s="98" t="s">
+      <c r="W6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="X6" s="96"/>
-      <c r="Y6" s="49"/>
+      <c r="X6" s="37"/>
+      <c r="Y6" s="15"/>
     </row>
     <row r="7" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="60" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="61" t="s">
+      <c r="H7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="62" t="s">
+      <c r="I7" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="60" t="s">
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="61" t="s">
+      <c r="M7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="62" t="s">
+      <c r="N7" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="O7" s="46"/>
-      <c r="P7" s="46"/>
-      <c r="Q7" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="R7" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="S7" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="T7" s="49"/>
-      <c r="U7" s="49"/>
-      <c r="V7" s="60" t="s">
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="R7" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="S7" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="W7" s="61" t="s">
+      <c r="W7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="X7" s="62" t="s">
+      <c r="X7" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="Y7" s="49"/>
+      <c r="Y7" s="15"/>
     </row>
     <row r="8" spans="1:29" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
-      <c r="B8" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="M8" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="N8" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="O8" s="46"/>
-      <c r="P8" s="46"/>
-      <c r="Q8" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="R8" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="S8" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="T8" s="49"/>
-      <c r="U8" s="49"/>
-      <c r="V8" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="W8" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="X8" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y8" s="49"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="S8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="W8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="X8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="15"/>
     </row>
     <row r="9" spans="1:29" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="46"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="49"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="46"/>
-      <c r="Q9" s="49"/>
-      <c r="R9" s="49"/>
-      <c r="S9" s="49"/>
-      <c r="T9" s="49"/>
-      <c r="U9" s="49"/>
-      <c r="V9" s="49"/>
-      <c r="W9" s="49"/>
-      <c r="X9" s="49"/>
-      <c r="Y9" s="46"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="12"/>
       <c r="Z9"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="49"/>
-      <c r="N10" s="49"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="49"/>
-      <c r="R10" s="49"/>
-      <c r="S10" s="49"/>
-      <c r="T10" s="49"/>
-      <c r="U10" s="49"/>
-      <c r="V10" s="49"/>
-      <c r="W10" s="49"/>
-      <c r="X10" s="49"/>
-      <c r="Y10" s="46"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="12"/>
       <c r="Z10"/>
     </row>
     <row r="11" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="39" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="33" t="s">
+      <c r="H11" s="66"/>
+      <c r="I11" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="30" t="s">
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="40"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="46"/>
-      <c r="Q11" s="46"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
       <c r="R11" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="S11" s="46"/>
-      <c r="T11" s="46"/>
-      <c r="U11" s="46"/>
-      <c r="V11" s="30" t="s">
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="W11" s="15" t="s">
+      <c r="W11" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="X11" s="40"/>
-      <c r="Y11" s="46"/>
+      <c r="X11" s="68"/>
+      <c r="Y11" s="12"/>
       <c r="Z11"/>
     </row>
     <row r="12" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="46"/>
-      <c r="B12" s="12" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="26" t="s">
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="N12" s="16" t="s">
+      <c r="H12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="62"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="O12" s="46"/>
-      <c r="P12" s="46"/>
-      <c r="Q12" s="12" t="s">
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="R12" s="47" t="s">
+      <c r="R12" s="13" t="s">
         <v>12</v>
       </c>
       <c r="S12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="T12" s="46"/>
-      <c r="U12" s="46"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="X12" s="16" t="s">
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="X12" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="Y12" s="46"/>
+      <c r="Y12" s="12"/>
       <c r="Z12"/>
     </row>
     <row r="13" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="46"/>
-      <c r="B13" s="46"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="21" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="34"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="46"/>
-      <c r="L13" s="35" t="s">
+      <c r="I13" s="64"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="M13" s="17"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="46"/>
-      <c r="Q13" s="46"/>
+      <c r="M13" s="42"/>
+      <c r="N13" s="58"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
       <c r="R13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="S13" s="46"/>
-      <c r="T13" s="46"/>
-      <c r="U13" s="46"/>
-      <c r="V13" s="35" t="s">
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="W13" s="17"/>
-      <c r="X13" s="31"/>
-      <c r="Y13" s="46"/>
+      <c r="W13" s="42"/>
+      <c r="X13" s="58"/>
+      <c r="Y13" s="12"/>
       <c r="Z13"/>
     </row>
     <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="49"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="46"/>
-      <c r="Q14" s="49"/>
-      <c r="R14" s="49"/>
-      <c r="S14" s="49"/>
-      <c r="T14" s="50"/>
-      <c r="U14" s="50"/>
-      <c r="V14" s="49"/>
-      <c r="W14" s="49"/>
-      <c r="X14" s="49"/>
-      <c r="Y14" s="46"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="12"/>
       <c r="Z14"/>
     </row>
     <row r="15" spans="1:29" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="46"/>
-      <c r="B15" s="63" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="94"/>
-      <c r="H15" s="69" t="s">
+      <c r="C15" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46"/>
-      <c r="L15" s="63" t="s">
+      <c r="I15" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="M15" s="69" t="s">
+      <c r="M15" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="O15" s="46"/>
-      <c r="P15" s="46"/>
-      <c r="Q15" s="63" t="s">
+      <c r="N15" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="R15" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="S15" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="T15" s="50"/>
-      <c r="U15" s="46"/>
-      <c r="V15" s="63" t="s">
+      <c r="R15" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="S15" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="T15" s="16"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="W15" s="69" t="s">
+      <c r="W15" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="X15" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y15" s="46"/>
+      <c r="X15" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y15" s="12"/>
       <c r="Z15"/>
     </row>
     <row r="16" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="46"/>
-      <c r="B16" s="66" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="92" t="s">
+      <c r="C16" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="61" t="s">
+      <c r="H16" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="95" t="s">
+      <c r="I16" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="M16" s="61" t="s">
+      <c r="M16" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="N16" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="O16" s="46"/>
-      <c r="P16" s="46"/>
-      <c r="Q16" s="66" t="s">
+      <c r="N16" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="R16" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="S16" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="T16" s="50"/>
-      <c r="U16" s="46"/>
-      <c r="V16" s="95" t="s">
+      <c r="R16" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="S16" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="T16" s="16"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="W16" s="61" t="s">
+      <c r="W16" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="X16" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y16" s="46"/>
+      <c r="X16" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y16" s="12"/>
       <c r="Z16"/>
     </row>
     <row r="17" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="46"/>
-      <c r="B17" s="67" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="68" t="s">
+      <c r="C17" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="70" t="s">
+      <c r="H17" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46"/>
-      <c r="L17" s="93"/>
-      <c r="M17" s="70" t="s">
+      <c r="I17" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="76"/>
+      <c r="M17" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="N17" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="67" t="s">
+      <c r="N17" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="R17" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="S17" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="T17" s="50"/>
-      <c r="U17" s="46"/>
-      <c r="V17" s="93"/>
-      <c r="W17" s="70" t="s">
+      <c r="R17" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="S17" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="T17" s="16"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="76"/>
+      <c r="W17" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="X17" s="59" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y17" s="46"/>
+      <c r="X17" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y17" s="12"/>
       <c r="Z17"/>
     </row>
     <row r="18" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="49"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="46"/>
-      <c r="Q18" s="49"/>
-      <c r="R18" s="49"/>
-      <c r="S18" s="49"/>
-      <c r="T18" s="49"/>
-      <c r="U18" s="49"/>
-      <c r="V18" s="49"/>
-      <c r="W18" s="49"/>
-      <c r="X18" s="49"/>
-      <c r="Y18" s="46"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="12"/>
       <c r="Z18"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="46"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
       <c r="P19"/>
       <c r="Q19"/>
       <c r="R19"/>
@@ -5040,31 +5029,31 @@
       <c r="Z19"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="46"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="39" t="s">
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="33" t="s">
+      <c r="H20" s="66"/>
+      <c r="I20" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
-      <c r="L20" s="41" t="s">
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="M20" s="15" t="s">
+      <c r="M20" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="N20" s="40"/>
-      <c r="O20" s="46"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="12"/>
       <c r="P20"/>
       <c r="Q20"/>
       <c r="R20"/>
@@ -5078,35 +5067,35 @@
       <c r="Z20"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="13" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="20" t="s">
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="N21" s="16" t="s">
+      <c r="H21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="62"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="O21" s="46"/>
+      <c r="O21" s="12"/>
       <c r="P21"/>
       <c r="Q21"/>
       <c r="R21"/>
@@ -5120,27 +5109,27 @@
       <c r="Z21"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="46"/>
-      <c r="B22" s="46"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="46"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="27" t="s">
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I22" s="43"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
-      <c r="L22" s="42" t="s">
+      <c r="I22" s="48"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="M22" s="28"/>
-      <c r="N22" s="31"/>
-      <c r="O22" s="46"/>
+      <c r="M22" s="54"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="12"/>
       <c r="P22"/>
       <c r="Q22"/>
       <c r="R22"/>
@@ -5154,21 +5143,21 @@
       <c r="Z22"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="46"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="49"/>
-      <c r="O23" s="46"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="12"/>
       <c r="P23"/>
       <c r="Q23"/>
       <c r="R23"/>
@@ -5182,39 +5171,39 @@
       <c r="Z23"/>
     </row>
     <row r="24" spans="1:26" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="46"/>
-      <c r="B24" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="I24" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
-      <c r="L24" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="M24" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="N24" s="65" t="s">
-        <v>12</v>
-      </c>
-      <c r="O24" s="46"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="M24" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="N24" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24" s="12"/>
       <c r="P24"/>
       <c r="Q24"/>
       <c r="R24"/>
@@ -5228,39 +5217,39 @@
       <c r="Z24"/>
     </row>
     <row r="25" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="46"/>
-      <c r="B25" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="60" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="61" t="s">
+      <c r="H25" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I25" s="62" t="s">
+      <c r="I25" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
-      <c r="L25" s="60" t="s">
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="M25" s="61" t="s">
+      <c r="M25" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="N25" s="62" t="s">
+      <c r="N25" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="O25" s="46"/>
+      <c r="O25" s="12"/>
       <c r="P25"/>
       <c r="Q25"/>
       <c r="R25"/>
@@ -5274,35 +5263,35 @@
       <c r="Z25"/>
     </row>
     <row r="26" spans="1:26" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="46"/>
-      <c r="B26" s="72" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="73" t="s">
+      <c r="C26" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="74" t="s">
+      <c r="D26" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="89" t="s">
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="93"/>
+      <c r="H26" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="74" t="s">
+      <c r="I26" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
-      <c r="L26" s="72" t="s">
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="M26" s="90" t="s">
+      <c r="M26" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="N26" s="88"/>
-      <c r="O26" s="46"/>
+      <c r="N26" s="96"/>
+      <c r="O26" s="12"/>
       <c r="P26"/>
       <c r="Q26"/>
       <c r="R26"/>
@@ -5316,21 +5305,21 @@
       <c r="Z26"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="46"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="49"/>
-      <c r="O27" s="46"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="15"/>
+      <c r="O27" s="12"/>
       <c r="P27"/>
       <c r="Q27"/>
       <c r="R27"/>
@@ -5344,21 +5333,21 @@
       <c r="Z27"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="46"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49"/>
-      <c r="O28" s="46"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+      <c r="O28" s="12"/>
       <c r="P28"/>
       <c r="Q28"/>
       <c r="R28"/>
@@ -5372,31 +5361,31 @@
       <c r="Z28"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A29" s="46"/>
-      <c r="B29" s="46"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="39" t="s">
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="38" t="s">
+      <c r="H29" s="66"/>
+      <c r="I29" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="J29" s="46"/>
-      <c r="K29" s="46"/>
-      <c r="L29" s="41" t="s">
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="M29" s="15" t="s">
+      <c r="M29" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="N29" s="40"/>
-      <c r="O29" s="46"/>
+      <c r="N29" s="68"/>
+      <c r="O29" s="12"/>
       <c r="P29"/>
       <c r="Q29"/>
       <c r="R29"/>
@@ -5410,200 +5399,200 @@
       <c r="Z29"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="46"/>
+      <c r="A30" s="12"/>
       <c r="B30" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" s="13" t="s">
+      <c r="C30" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="20" t="s">
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="I30" s="24"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="46"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="N30" s="25" t="s">
+      <c r="H30" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="85"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="N30" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="O30" s="46"/>
+      <c r="O30" s="12"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="46"/>
-      <c r="B31" s="46"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D31" s="46"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="46"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="21" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="I31" s="34"/>
-      <c r="J31" s="46"/>
-      <c r="K31" s="46"/>
-      <c r="L31" s="35" t="s">
+      <c r="I31" s="64"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="M31" s="17"/>
-      <c r="N31" s="37"/>
-      <c r="O31" s="46"/>
+      <c r="M31" s="42"/>
+      <c r="N31" s="87"/>
+      <c r="O31" s="12"/>
     </row>
     <row r="32" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="46"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="46"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="49"/>
-      <c r="O32" s="46"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="12"/>
     </row>
     <row r="33" spans="1:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="46"/>
-      <c r="B33" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="64" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="75" t="s">
+      <c r="A33" s="12"/>
+      <c r="B33" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="69" t="s">
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="78" t="s">
+      <c r="I33" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="M33" s="69" t="s">
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="M33" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="N33" s="87"/>
-      <c r="O33" s="46"/>
+      <c r="N33" s="88"/>
+      <c r="O33" s="12"/>
     </row>
     <row r="34" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
-      <c r="B34" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="55" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="76" t="s">
+      <c r="A34" s="12"/>
+      <c r="B34" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="61" t="s">
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I34" s="86" t="s">
+      <c r="I34" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="J34" s="46"/>
-      <c r="K34" s="46"/>
-      <c r="L34" s="54" t="s">
-        <v>12</v>
-      </c>
-      <c r="M34" s="61" t="s">
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="M34" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="N34" s="85" t="s">
+      <c r="N34" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="O34" s="46"/>
+      <c r="O34" s="12"/>
     </row>
     <row r="35" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="46"/>
-      <c r="B35" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="58" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="77" t="s">
+      <c r="A35" s="12"/>
+      <c r="B35" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="70" t="s">
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="I35" s="84"/>
-      <c r="J35" s="46"/>
-      <c r="K35" s="46"/>
-      <c r="L35" s="57" t="s">
-        <v>12</v>
-      </c>
-      <c r="M35" s="70" t="s">
+      <c r="I35" s="83"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="M35" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="N35" s="77" t="s">
+      <c r="N35" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="O35" s="46"/>
+      <c r="O35" s="12"/>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="46"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="49"/>
-      <c r="N36" s="49"/>
-      <c r="O36" s="46"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="12"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
       <c r="K37"/>
       <c r="L37"/>
       <c r="M37"/>
@@ -5611,13 +5600,13 @@
       <c r="O37"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F38" s="46"/>
-      <c r="G38" s="46"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
       <c r="H38" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I38" s="46"/>
-      <c r="J38" s="46"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
       <c r="K38"/>
       <c r="L38"/>
       <c r="M38"/>
@@ -5625,17 +5614,17 @@
       <c r="O38"/>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F39" s="46"/>
-      <c r="G39" s="79" t="s">
+      <c r="F39" s="12"/>
+      <c r="G39" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H39" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="I39" s="13" t="s">
+      <c r="H39" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I39" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="J39" s="46"/>
+      <c r="J39" s="12"/>
       <c r="K39"/>
       <c r="L39"/>
       <c r="M39"/>
@@ -5643,13 +5632,13 @@
       <c r="O39"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
       <c r="H40" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I40" s="46"/>
-      <c r="J40" s="46"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
       <c r="K40"/>
       <c r="L40"/>
       <c r="M40"/>
@@ -5657,11 +5646,11 @@
       <c r="O40"/>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F41" s="46"/>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46"/>
-      <c r="I41" s="46"/>
-      <c r="J41" s="46"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
       <c r="K41"/>
       <c r="L41"/>
       <c r="M41"/>
@@ -5669,93 +5658,94 @@
       <c r="O41"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F42" s="46"/>
-      <c r="G42" s="44" t="s">
+      <c r="F42" s="12"/>
+      <c r="G42" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H42" s="18"/>
-      <c r="I42" s="38" t="s">
+      <c r="H42" s="44"/>
+      <c r="I42" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="J42" s="46"/>
+      <c r="J42" s="12"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F43" s="46"/>
-      <c r="G43" s="82" t="s">
+      <c r="F43" s="12"/>
+      <c r="G43" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="H43" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="I43" s="24"/>
-      <c r="J43" s="46"/>
+      <c r="H43" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I43" s="85"/>
+      <c r="J43" s="12"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F44" s="46"/>
-      <c r="G44" s="83"/>
-      <c r="H44" s="27" t="s">
+      <c r="F44" s="12"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="I44" s="43"/>
-      <c r="J44" s="46"/>
+      <c r="I44" s="91"/>
+      <c r="J44" s="12"/>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F45" s="46"/>
-      <c r="G45" s="46"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F46" s="46"/>
-      <c r="G46" s="80" t="s">
+      <c r="F46" s="12"/>
+      <c r="G46" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="H46" s="29" t="s">
+      <c r="H46" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="I46" s="45"/>
-      <c r="J46" s="46"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="12"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F47" s="46"/>
-      <c r="G47" s="81"/>
-      <c r="H47" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="I47" s="25" t="s">
+      <c r="F47" s="12"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I47" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="J47" s="46"/>
+      <c r="J47" s="12"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F48" s="46"/>
-      <c r="G48" s="42" t="s">
+      <c r="F48" s="12"/>
+      <c r="G48" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="H48" s="28"/>
-      <c r="I48" s="37"/>
-      <c r="J48" s="46"/>
+      <c r="H48" s="54"/>
+      <c r="I48" s="87"/>
+      <c r="J48" s="12"/>
     </row>
     <row r="49" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F49" s="46"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="49"/>
-      <c r="I49" s="49"/>
-      <c r="J49" s="46"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="V13:W13"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="I47:I48"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="V11:V12"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="X12:X13"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="V2:W2"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="G2:H2"/>
@@ -5763,19 +5753,29 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="L4:M4"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="I47:I48"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="L2:L3"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="I20:I21"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="L20:L21"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="N21:N22"/>
     <mergeCell ref="L22:M22"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="L29:L30"/>
+    <mergeCell ref="V13:W13"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="N21:N22"/>
     <mergeCell ref="M29:N29"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="I29:I30"/>
@@ -5783,17 +5783,6 @@
     <mergeCell ref="G30:G31"/>
     <mergeCell ref="L31:M31"/>
     <mergeCell ref="H31:I31"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="V11:V12"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="X12:X13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="66" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>